<commit_message>
Data Cleaning of GEIH
year 2015.01-2023.07. With this notebook we can clean the previous years as well in order to build our historical data.
</commit_message>
<xml_diff>
--- a/Datasets/List of Possible Data Sets.xlsx
+++ b/Datasets/List of Possible Data Sets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dda39ef004021ca5/Desktop/MDS 2024/Master Thesis/Datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dda39ef004021ca5/Documents/GitHub/Hertie_School_MDS_Master_Thesis/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{3161AA99-2E20-4B85-8449-7A266E90B51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C26B438D-2980-4652-BC6F-0A4D552D6201}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{3161AA99-2E20-4B85-8449-7A266E90B51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48016AFD-F86B-469A-9FAB-8999C0DFD13B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1E935717-DD72-45D7-9C68-C9ACEFDD9922}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Bases de Datos Tesis</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -99,13 +96,46 @@
   </si>
   <si>
     <t>Evolution of % of workers by contract type</t>
+  </si>
+  <si>
+    <t>https://www.dane.gov.co/index.php/estadisticas-por-tema/demografia-y-poblacion/proyecciones-de-poblacion</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>DCD-area-proypoblacion-Mun-1985-2024-(Population Evolution of Cities)</t>
+  </si>
+  <si>
+    <t>1984-2035</t>
+  </si>
+  <si>
+    <t>GEIH_cleaned_2015-01-2023-07</t>
+  </si>
+  <si>
+    <t>https://www.dane.gov.co/index.php/estadisticas-por-tema/mercado-laboral/empleo-y-desempleo/mercado-laboral-historicos</t>
+  </si>
+  <si>
+    <t>DANE</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>2015.01-2023.07</t>
+  </si>
+  <si>
+    <t>Yes (missing previous years)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +147,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -256,14 +294,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -275,7 +313,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -288,47 +325,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -341,12 +394,11 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -359,8 +411,22 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -475,15 +541,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A23D101-2A44-4089-BD97-FEA86080D220}" name="Tabla1" displayName="Tabla1" ref="A3:F17" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A3:F17" xr:uid="{4A23D101-2A44-4089-BD97-FEA86080D220}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{845D20C5-CB1A-4C08-8F4E-F55FF1563C33}" name="Title" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{BFEB8C7B-6C34-415A-AA17-36DE8B43DE06}" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{BA9788FE-8840-43CF-B4CD-9FEBE6CD81DA}" name="Source" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1A710DD9-8D66-4BE4-88A3-A246CFAF52F1}" name="Timeframe" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{91E3C52F-3D0A-4235-9BC1-B39917C7C053}" name="Got it?" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{40A9E45C-440D-4F5E-8EDB-7646D73F4F58}" name="Cleaned?" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A23D101-2A44-4089-BD97-FEA86080D220}" name="Tabla1" displayName="Tabla1" ref="A1:G15" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:G15" xr:uid="{4A23D101-2A44-4089-BD97-FEA86080D220}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{845D20C5-CB1A-4C08-8F4E-F55FF1563C33}" name="Title" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{BFEB8C7B-6C34-415A-AA17-36DE8B43DE06}" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{F40FC73B-648C-470A-AACA-558D783A5F8B}" name="Source" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{BA9788FE-8840-43CF-B4CD-9FEBE6CD81DA}" name="Link" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1A710DD9-8D66-4BE4-88A3-A246CFAF52F1}" name="Timeframe" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{91E3C52F-3D0A-4235-9BC1-B39917C7C053}" name="Got it?" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{40A9E45C-440D-4F5E-8EDB-7646D73F4F58}" name="Cleaned?" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -786,188 +853,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD5FE44-E603-43A6-A941-8DC122599DDB}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="2" max="2" width="71.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="12" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="13" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="13" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="13" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{E54AA009-5C77-4AE8-8A9A-41A014D22DBA}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{E2D73C58-1A1C-4D25-AFC1-85ECBD970296}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>